<commit_message>
Daily Srum update, User Case Map verbessert
</commit_message>
<xml_diff>
--- a/Daily_Scrum.xlsx
+++ b/Daily_Scrum.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F042D554-1DB5-421F-96A3-191C4A9D0DBE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E748FD-1178-4EFE-BAE0-50125FD4C65F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="28">
   <si>
     <t>Datum</t>
   </si>
@@ -223,6 +223,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -235,10 +239,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -523,7 +523,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K18" sqref="K18"/>
+      <selection pane="topRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -552,42 +552,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="11" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="11" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="11" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="11" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="13"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="15"/>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="14"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
@@ -829,7 +829,7 @@
       <c r="N7" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="12" t="s">
         <v>25</v>
       </c>
       <c r="R7" t="s">
@@ -902,7 +902,7 @@
       <c r="M10" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="11" t="s">
         <v>17</v>
       </c>
       <c r="R10" t="s">
@@ -937,7 +937,7 @@
       <c r="M11" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="R11" t="s">
@@ -983,7 +983,7 @@
       <c r="A13" s="3">
         <v>43175</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
@@ -1062,11 +1062,17 @@
       <c r="N16" t="s">
         <v>10</v>
       </c>
+      <c r="Q16" t="s">
+        <v>25</v>
+      </c>
       <c r="R16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="U16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>43181</v>
       </c>
@@ -1082,11 +1088,17 @@
       <c r="N17" t="s">
         <v>10</v>
       </c>
+      <c r="Q17" t="s">
+        <v>25</v>
+      </c>
       <c r="R17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="U17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>43182</v>
       </c>
@@ -1099,11 +1111,20 @@
       <c r="J18" t="s">
         <v>10</v>
       </c>
+      <c r="M18" t="s">
+        <v>24</v>
+      </c>
       <c r="N18" t="s">
         <v>10</v>
       </c>
+      <c r="Q18" t="s">
+        <v>25</v>
+      </c>
       <c r="R18" t="s">
         <v>10</v>
+      </c>
+      <c r="U18" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>